<commit_message>
- update of existing permission tests for class roster tool - updated test site and updated test data to reflect the ACP criteria in TLT-2650: https://docs.google.com/spreadsheets/d/15RmyBBSzc9YkrZUlhHcAWWgRRZLzET-S3AHIzme4q-0/edit#gid=0
</commit_message>
<xml_diff>
--- a/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
+++ b/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hic048/projects/canvas_manage_course/selenium_tests/class_roster/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="51200" yWindow="13940" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
-    <sheet name="Site Setup" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Site Setup" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
   <si>
     <t xml:space="preserve">Roles </t>
   </si>
@@ -32,9 +36,6 @@
     <t xml:space="preserve">Guest </t>
   </si>
   <si>
-    <t>Harvard-Viewer</t>
-  </si>
-  <si>
     <t>Observer</t>
   </si>
   <si>
@@ -110,9 +111,6 @@
     <t>test7@mcelroy.org</t>
   </si>
   <si>
-    <t>test8@mcelroy.org</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -122,28 +120,149 @@
     <t xml:space="preserve">canvas_user_id </t>
   </si>
   <si>
-    <t>Access to CLASS ROSTER</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Course Level Role (course 3787) </t>
   </si>
   <si>
-    <t xml:space="preserve">Site Under Test </t>
-  </si>
-  <si>
-    <t>https://canvas.dev.tlt.harvard.edu/courses/3787/external_tools/162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Data Info: </t>
-  </si>
-  <si>
-    <t>https://confluence.huit.harvard.edu/display/TLT/SIS+Import+of+Test+Data+for+Selenium+Permissions+Test</t>
-  </si>
-  <si>
     <t>92234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA </t>
+  </si>
+  <si>
+    <t>92242</t>
+  </si>
+  <si>
+    <t>92229</t>
+  </si>
+  <si>
+    <t>Course Head</t>
+  </si>
+  <si>
+    <t>92230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course Support Staff </t>
+  </si>
+  <si>
+    <t>92239</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>90675</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faculty </t>
+  </si>
+  <si>
+    <t>92238</t>
+  </si>
+  <si>
+    <t>92232</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>92237</t>
+  </si>
+  <si>
+    <t>Prospective Enrollee</t>
+  </si>
+  <si>
+    <t>92236</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>92259</t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t>90670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School Liaison </t>
+  </si>
+  <si>
+    <t>92258</t>
+  </si>
+  <si>
+    <t>Department Admin</t>
+  </si>
+  <si>
+    <t>92260</t>
+  </si>
+  <si>
+    <t>Helpdesk</t>
+  </si>
+  <si>
+    <t>92261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Observer </t>
+  </si>
+  <si>
+    <t>92295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Admin </t>
+  </si>
+  <si>
+    <t>test12@mcelroy.org</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>test13@mcelroy.org</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>test10@mcelroy.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student </t>
+  </si>
+  <si>
+    <t>test9@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test34@mcelroy.org</t>
+  </si>
+  <si>
+    <t>test36@mcelroy.org</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Level role (sub-account 10) </t>
+  </si>
+  <si>
+    <t>test37@mcelroy.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Librarian </t>
+  </si>
+  <si>
+    <t>test35@mcelroy.org</t>
+  </si>
+  <si>
+    <t>Access to Class Roster
+for COLGSAS</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>role</t>
   </si>
 </sst>
 </file>
@@ -386,16 +505,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="129" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
   </cellXfs>
   <cellStyles count="163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -564,6 +686,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -889,276 +1016,545 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
+      <c r="C14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="31" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18" style="3" customWidth="1"/>
+    <col min="4" max="4" width="32" style="3" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
+        <v>92241</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>92242</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>92229</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>92230</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3">
+        <v>92239</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3">
+        <v>90675</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4">
-        <v>92241</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
-        <v>92242</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>92229</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3">
+        <v>92238</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
-        <v>92230</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="C9" s="3">
         <v>92232</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
+      <c r="D9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3">
+        <v>92234</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="3">
+        <v>92237</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="3">
+        <v>92236</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>92295</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4">
-        <v>92295</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="C15" s="3">
+        <v>90670</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4">
-        <v>90670</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4">
-        <v>92238</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4">
-        <v>92234</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4">
-        <v>92235</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="3">
+        <v>92258</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="3">
+        <v>92260</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="3">
+        <v>92261</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="3">
+        <v>92259</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1167,38 +1563,20 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B14" r:id="rId6"/>
+    <hyperlink ref="B15" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B8" r:id="rId9"/>
+    <hyperlink ref="B6" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="B17" r:id="rId12"/>
+    <hyperlink ref="B19" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
+    <hyperlink ref="B12" r:id="rId15"/>
+    <hyperlink ref="B11" r:id="rId16"/>
+    <hyperlink ref="B18" r:id="rId17"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ok, fixed code and data issues.
</commit_message>
<xml_diff>
--- a/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
+++ b/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="13940" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="16780" yWindow="29260" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="80">
   <si>
     <t xml:space="preserve">Roles </t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t xml:space="preserve">Course or Account Level Roles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes </t>
   </si>
   <si>
     <t>Email</t>
@@ -263,6 +260,12 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/15RmyBBSzc9YkrZUlhHcAWWgRRZLzET-S3AHIzme4q-0/edit#gid=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Based on TLT-2650: </t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,32 +1034,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
@@ -1064,54 +1067,54 @@
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
@@ -1119,10 +1122,10 @@
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
@@ -1130,101 +1133,101 @@
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1235,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1256,13 +1259,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>19</v>
@@ -1279,10 +1282,10 @@
         <v>92241</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,10 +1299,10 @@
         <v>92242</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,10 +1316,10 @@
         <v>92229</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,44 +1333,44 @@
         <v>92230</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3">
         <v>92239</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="C7" s="3">
         <v>90675</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,15 +1384,15 @@
         <v>92238</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>10</v>
@@ -1398,10 +1401,10 @@
         <v>92232</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,55 +1412,55 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <v>92234</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3">
         <v>92237</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="C12" s="3">
         <v>92236</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>17</v>
@@ -1466,15 +1469,15 @@
         <v>92295</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>18</v>
@@ -1483,78 +1486,88 @@
         <v>90670</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3">
         <v>92258</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3">
         <v>92260</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3">
         <v>92261</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="C19" s="3">
         <v>92259</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- inaccurate text cleanup - data update
</commit_message>
<xml_diff>
--- a/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
+++ b/selenium_tests/class_roster/test_data/class_roster_roles_access.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="29260" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="15060" yWindow="29260" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1070,7 +1070,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>35</v>

</xml_diff>